<commit_message>
Prepare seed data (except for shipment part (no relationships) and hashing, make adjustments in .xlsx test-data files
</commit_message>
<xml_diff>
--- a/Persistence/Database/test-data/Couriers.xlsx
+++ b/Persistence/Database/test-data/Couriers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vieva\Desktop\PSK\komandinis\shipping-service\Persistence\Database\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8411D66A-1956-496B-9652-2F1961B9AE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2253BA-F944-4C60-8B93-4F2E60593B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{16951523-755D-4673-83F3-901F0B7B3088}"/>
   </bookViews>
@@ -497,7 +497,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="D11" sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,10 +512,10 @@
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -526,10 +526,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -540,10 +540,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -554,10 +554,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -568,10 +568,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>12</v>
@@ -582,10 +582,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>4</v>
@@ -596,10 +596,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -610,10 +610,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>5</v>
@@ -624,10 +624,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>10</v>
@@ -637,11 +637,11 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1">
         <v>125521</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>9</v>
@@ -652,10 +652,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>21</v>

</xml_diff>